<commit_message>
add user Reviews Table
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7031A880-3E43-4BF1-A804-9212AEFD7BC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{571995E2-BBA3-47D1-97E2-11B2D93E836D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="23310" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="23340" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
   <si>
     <t>Table Name</t>
   </si>
@@ -159,12 +159,6 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>parking_meter</t>
-  </si>
-  <si>
-    <t>parking_meter_id</t>
-  </si>
-  <si>
     <t>per_hr_charges</t>
   </si>
   <si>
@@ -331,6 +325,33 @@
   </si>
   <si>
     <t>only 1 vehicle can be an default vehicle of a user.</t>
+  </si>
+  <si>
+    <t>default value should be inactive. After verification parking location will be active</t>
+  </si>
+  <si>
+    <t>parking_details</t>
+  </si>
+  <si>
+    <t>parking_details_id</t>
+  </si>
+  <si>
+    <t>parking_reviews</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>rating range will be from 1 to 5</t>
+  </si>
+  <si>
+    <t>user_Id</t>
+  </si>
+  <si>
+    <t>reviews_Text</t>
+  </si>
+  <si>
+    <t>parking_id</t>
   </si>
 </sst>
 </file>
@@ -696,10 +717,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -707,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -715,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -723,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -731,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -739,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -747,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -755,7 +776,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -765,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:G136"/>
+  <dimension ref="C1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,12 +939,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>27</v>
       </c>
@@ -931,41 +952,41 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" t="s">
         <v>100</v>
       </c>
-      <c r="E28" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>3</v>
       </c>
@@ -973,32 +994,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1006,17 +1027,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1024,22 +1045,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>42</v>
       </c>
@@ -1047,399 +1068,439 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
         <v>52</v>
       </c>
-      <c r="F70" t="s">
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="74" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="75" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>54</v>
-      </c>
-      <c r="E76" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
+      <c r="E89" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
         <v>56</v>
       </c>
-      <c r="E80" t="s">
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="81" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+      <c r="E92" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
+    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>62</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>59</v>
-      </c>
-      <c r="E83" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="85" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="86" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="87" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
-        <v>64</v>
-      </c>
-      <c r="E87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>67</v>
+      </c>
+      <c r="E112" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="97" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C100" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="101" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D101" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="102" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D102" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D103" t="s">
-        <v>69</v>
-      </c>
-      <c r="E103" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="104" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D104" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="105" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D105" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="106" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D106" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="107" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D107" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="108" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C111" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="112" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D112" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D113" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D114" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
         <v>9</v>
       </c>
       <c r="E115" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="116" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="117" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C119" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="120" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D120" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="121" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
         <v>9</v>
       </c>
-      <c r="E122" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="123" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D123" t="s">
-        <v>69</v>
-      </c>
-      <c r="E123" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="124" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D124" t="s">
+      <c r="E124" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="125" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D125" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="126" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>67</v>
+      </c>
+      <c r="E132" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="139" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>3</v>
+      </c>
+      <c r="E139" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="140" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D129" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="130" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D130" t="s">
-        <v>3</v>
-      </c>
-      <c r="E130" t="s">
+    <row r="141" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="131" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D131" t="s">
+      <c r="E141" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="132" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D132" t="s">
+    <row r="142" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
         <v>83</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E142" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="133" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D133" t="s">
+    <row r="143" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
         <v>85</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E143" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="134" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D134" t="s">
+    <row r="144" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
         <v>87</v>
       </c>
-      <c r="E134" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="135" spans="3:7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D135" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="136" spans="3:7" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add parking Loc by Agent
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7B7F3DEE-8042-43C4-81C1-A5D0DBD54A39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7D303E6B-58A1-4ED2-A767-AFD29EBC91C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="23370" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="23400" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>Table Name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>open_time</t>
   </si>
   <si>
-    <t>closed_time</t>
-  </si>
-  <si>
     <t>vehicle_name</t>
   </si>
   <si>
@@ -349,6 +346,12 @@
   </si>
   <si>
     <t>monthly_rate</t>
+  </si>
+  <si>
+    <t>close_time</t>
+  </si>
+  <si>
+    <t>capacity</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -725,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -733,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -749,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -757,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -765,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -773,7 +776,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -783,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:G144"/>
+  <dimension ref="C1:G146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,13 +954,13 @@
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
         <v>96</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>97</v>
-      </c>
-      <c r="G28" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
@@ -972,12 +975,12 @@
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
@@ -1052,452 +1055,459 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>42</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E51" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="52" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
         <v>44</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="58" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="66" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    <row r="69" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="70" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="73" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>102</v>
+      </c>
+      <c r="F73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="79" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+      <c r="F80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
+    <row r="84" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>51</v>
+      </c>
+      <c r="E90" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>54</v>
+      </c>
+      <c r="E93" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>59</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
+    <row r="99" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="102" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="111" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>48</v>
-      </c>
-      <c r="F79" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>50</v>
-      </c>
-      <c r="E85" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>52</v>
-      </c>
-      <c r="E89" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D90" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
+      <c r="E113" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="123" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>55</v>
-      </c>
-      <c r="E92" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>60</v>
-      </c>
-      <c r="E96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
+    <row r="124" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
+    <row r="128" spans="3:7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="133" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>64</v>
+      </c>
+      <c r="E133" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="135" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="139" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="140" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D110" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D111" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>65</v>
-      </c>
-      <c r="E112" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D114" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D115" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D121" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D122" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D123" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D124" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D129" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D131" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D132" t="s">
-        <v>65</v>
-      </c>
-      <c r="E132" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D133" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D135" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C137" t="s">
+      <c r="E140" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D138" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D139" t="s">
-        <v>3</v>
-      </c>
-      <c r="E139" t="s">
+    <row r="141" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D140" t="s">
+    <row r="142" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
+      <c r="E142" t="s">
         <v>79</v>
       </c>
-      <c r="E141" t="s">
+    </row>
+    <row r="143" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D142" t="s">
+      <c r="E143" t="s">
         <v>81</v>
       </c>
-      <c r="E142" t="s">
+    </row>
+    <row r="144" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D143" t="s">
+      <c r="E144" t="s">
         <v>83</v>
       </c>
-      <c r="E143" t="s">
+    </row>
+    <row r="145" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D144" t="s">
-        <v>85</v>
-      </c>
-    </row>
+    <row r="146" spans="3:7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Rating and Booking charges column
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7D303E6B-58A1-4ED2-A767-AFD29EBC91C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B6707ECD-4035-4587-92C5-989E74CBAA90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="23400" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="23430" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
   <si>
     <t>Table Name</t>
   </si>
@@ -352,6 +352,27 @@
   </si>
   <si>
     <t>capacity</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>// Avg Rating of this parking location</t>
+  </si>
+  <si>
+    <t>booking_rate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Favorite_parking</t>
+  </si>
+  <si>
+    <t>parking_name</t>
   </si>
 </sst>
 </file>
@@ -786,10 +807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:G146"/>
+  <dimension ref="C1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,20 +822,26 @@
     <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -824,8 +851,11 @@
       <c r="G4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>6</v>
       </c>
@@ -833,12 +863,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -846,7 +876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>11</v>
       </c>
@@ -854,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -862,7 +892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>15</v>
       </c>
@@ -870,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>16</v>
       </c>
@@ -878,55 +908,61 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>24</v>
       </c>
@@ -934,17 +970,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>27</v>
       </c>
@@ -952,7 +988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>95</v>
       </c>
@@ -963,22 +999,22 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>94</v>
       </c>
@@ -986,7 +1022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>3</v>
       </c>
@@ -994,50 +1030,53 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>34</v>
       </c>
       <c r="G42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>37</v>
       </c>
@@ -1045,32 +1084,32 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>42</v>
       </c>
@@ -1078,436 +1117,510 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>102</v>
+      </c>
+      <c r="G53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>44</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="55" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
+    <row r="56" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="59" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="58" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+      <c r="I59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="61" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="62" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="63" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="64" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="65" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
+    <row r="66" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
+    <row r="68" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
+    <row r="69" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+    <row r="72" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="70" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+      <c r="I72" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
+    <row r="74" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+    <row r="75" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
+    <row r="76" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
         <v>102</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F76" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
+    <row r="77" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
+    <row r="78" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="79" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>63</v>
+      </c>
+      <c r="I82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="79" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
+      <c r="I89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
+    <row r="91" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
         <v>47</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F91" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+    <row r="92" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="95" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="85" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
+      <c r="I95" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
+    <row r="97" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
         <v>49</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E97" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
+    <row r="98" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+    <row r="99" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
         <v>51</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E101" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
+    <row r="102" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
+    <row r="103" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
+    <row r="104" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
         <v>54</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E104" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
+    <row r="105" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
+    <row r="106" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
+    <row r="107" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
+    <row r="108" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
         <v>59</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E108" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
+    <row r="109" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D99" t="s">
+    <row r="110" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
+    <row r="113" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
+    <row r="114" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="104" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="105" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="106" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="111" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D111" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="112" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>64</v>
-      </c>
-      <c r="E113" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="114" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D114" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="118" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="122" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="123" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
+        <v>64</v>
+      </c>
+      <c r="E124" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
+    <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
         <v>9</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E136" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="126" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
+    <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D127" t="s">
+    <row r="138" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="3:7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
+    <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="130" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
+    <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D131" t="s">
+    <row r="142" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="132" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D132" t="s">
+    <row r="143" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
         <v>9</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="133" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D133" t="s">
+    <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
         <v>64</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E144" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="134" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
+    <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="135" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D135" t="s">
+    <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="136" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D136" t="s">
+    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C138" t="s">
+    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="139" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D139" t="s">
+    <row r="150" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D140" t="s">
+    <row r="151" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
         <v>3</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E151" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="141" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
+    <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D142" t="s">
+    <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
         <v>78</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E153" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="143" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D143" t="s">
+    <row r="154" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
         <v>80</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E154" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D144" t="s">
+    <row r="155" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
         <v>82</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E155" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="145" spans="3:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D145" t="s">
+    <row r="156" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="146" spans="3:7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add user wallet entity
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B6707ECD-4035-4587-92C5-989E74CBAA90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{24B8C198-BCC6-49E6-97BA-5EF0A7BED29A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="23430" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="23460" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>Table Name</t>
   </si>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
   <dimension ref="C1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,6 +1013,9 @@
       <c r="C32" t="s">
         <v>93</v>
       </c>
+      <c r="I32" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">

</xml_diff>

<commit_message>
Add park booking history entity
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{24B8C198-BCC6-49E6-97BA-5EF0A7BED29A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C9CAA5C9-58AE-49F9-8F57-60AEFBF41564}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="23460" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="23490" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="127">
   <si>
     <t>Table Name</t>
   </si>
@@ -204,9 +204,6 @@
     <t>user_wallet_status</t>
   </si>
   <si>
-    <t>purchase_trans_history</t>
-  </si>
-  <si>
     <t>purchase_trans_history_id</t>
   </si>
   <si>
@@ -303,12 +300,6 @@
     <t>Wallet adding</t>
   </si>
   <si>
-    <t>user_account</t>
-  </si>
-  <si>
-    <t>user_account_id</t>
-  </si>
-  <si>
     <t>is_default</t>
   </si>
   <si>
@@ -373,6 +364,45 @@
   </si>
   <si>
     <t>parking_name</t>
+  </si>
+  <si>
+    <t>user_wallet</t>
+  </si>
+  <si>
+    <t>this table is related to deposit money history</t>
+  </si>
+  <si>
+    <t>Park_Booking_History</t>
+  </si>
+  <si>
+    <t>Booking_Type</t>
+  </si>
+  <si>
+    <t>In_Time</t>
+  </si>
+  <si>
+    <t>Out_Time</t>
+  </si>
+  <si>
+    <t>// initial booking or fullpayment</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>user_purchase_trans_history</t>
+  </si>
+  <si>
+    <t>amt</t>
+  </si>
+  <si>
+    <t>Agent_trans_history</t>
+  </si>
+  <si>
+    <t>trans_type</t>
+  </si>
+  <si>
+    <t>//cr - dr</t>
   </si>
 </sst>
 </file>
@@ -738,10 +768,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -749,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -757,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -765,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -773,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -781,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -789,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -797,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -807,10 +837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:I157"/>
+  <dimension ref="C1:I177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -852,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -913,7 +943,7 @@
         <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
@@ -959,7 +989,7 @@
         <v>23</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -990,13 +1020,13 @@
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
@@ -1011,15 +1041,15 @@
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="I32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
@@ -1066,7 +1096,7 @@
         <v>35</v>
       </c>
       <c r="I42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
@@ -1109,7 +1139,7 @@
     </row>
     <row r="50" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1122,15 +1152,15 @@
     </row>
     <row r="52" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,7 +1168,7 @@
         <v>44</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1153,15 +1183,15 @@
     </row>
     <row r="59" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I59" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1171,12 +1201,12 @@
     </row>
     <row r="62" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1186,12 +1216,12 @@
     </row>
     <row r="65" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1211,20 +1241,20 @@
     </row>
     <row r="72" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I72" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1234,15 +1264,15 @@
     </row>
     <row r="76" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F76" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1254,15 +1284,15 @@
     <row r="80" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="81" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I82" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1277,7 +1307,7 @@
     </row>
     <row r="85" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1292,7 +1322,7 @@
         <v>45</v>
       </c>
       <c r="I89" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1318,7 +1348,7 @@
         <v>49</v>
       </c>
       <c r="I95" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1400,230 +1430,317 @@
         <v>13</v>
       </c>
     </row>
+    <row r="111" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="113" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>60</v>
+      <c r="D113" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="114" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>3</v>
+        <v>117</v>
+      </c>
+      <c r="F116" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>125</v>
+      </c>
+      <c r="F118" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="121" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
-        <v>62</v>
+      <c r="D121" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>64</v>
-      </c>
-      <c r="E124" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
-        <v>29</v>
-      </c>
-    </row>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D127" t="s">
-        <v>9</v>
-      </c>
-      <c r="E127" t="s">
-        <v>67</v>
+      <c r="C127" t="s">
+        <v>122</v>
+      </c>
+      <c r="F127" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="132" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D133" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
-        <v>3</v>
-      </c>
-    </row>
+      <c r="D132" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D135" t="s">
-        <v>70</v>
+      <c r="C135" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>63</v>
+      </c>
+      <c r="E138" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="140" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C140" t="s">
-        <v>71</v>
+      <c r="D140" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>70</v>
+        <v>9</v>
+      </c>
+      <c r="E141" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="142" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="143" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>9</v>
-      </c>
-      <c r="E143" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D144" t="s">
-        <v>64</v>
-      </c>
-      <c r="E144" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D145" t="s">
-        <v>66</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D146" t="s">
+      <c r="C146" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D147" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C149" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="150" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D150" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="151" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D151" t="s">
-        <v>3</v>
-      </c>
-      <c r="E151" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D152" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>78</v>
-      </c>
-      <c r="E153" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="154" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>80</v>
-      </c>
-      <c r="E154" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>82</v>
-      </c>
-      <c r="E155" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="156" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>9</v>
+      </c>
+      <c r="E156" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="158" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="162" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="163" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="164" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>63</v>
+      </c>
+      <c r="E164" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="166" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="167" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="170" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="171" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>3</v>
+      </c>
+      <c r="E171" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>77</v>
+      </c>
+      <c r="E173" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="174" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D174" t="s">
+        <v>79</v>
+      </c>
+      <c r="E174" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="175" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>81</v>
+      </c>
+      <c r="E175" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="176" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="177" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add vehicle Detail id in entity
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{926B27B3-2C5F-4928-BFB6-AD5333AA0A14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1ACEA3EC-1F6C-4EB2-8EE4-18243703B0BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="23580" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="23610" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
   <si>
     <t>Table Name</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>max_used_count</t>
+  </si>
+  <si>
+    <t>// Running , Cancel , Parked , Completed</t>
   </si>
 </sst>
 </file>
@@ -865,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:I206"/>
+  <dimension ref="C1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182:D189"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,440 +1481,455 @@
     </row>
     <row r="115" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>112</v>
-      </c>
-      <c r="F117" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F119" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>114</v>
+        <v>120</v>
+      </c>
+      <c r="F121" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="124" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="F124" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
+    <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D129" t="s">
-        <v>59</v>
-      </c>
-      <c r="I129" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>123</v>
+        <v>59</v>
+      </c>
+      <c r="I131" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="132" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C135" t="s">
+    <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D136" t="s">
-        <v>59</v>
-      </c>
-      <c r="I136" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D137" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="138" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>117</v>
+        <v>59</v>
+      </c>
+      <c r="I138" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>120</v>
-      </c>
-      <c r="F139" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>116</v>
+        <v>120</v>
+      </c>
+      <c r="F141" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="142" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>9</v>
-      </c>
-      <c r="E142" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
     </row>
     <row r="143" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
     </row>
     <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
+        <v>9</v>
+      </c>
+      <c r="E144" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C147" t="s">
+    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D148" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D149" t="s">
-        <v>3</v>
-      </c>
-      <c r="I149" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="150" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
     </row>
     <row r="151" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>120</v>
+        <v>3</v>
+      </c>
+      <c r="I151" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="154" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
     </row>
     <row r="155" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="159" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="160" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C161" t="s">
+    <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="162" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D162" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="163" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D163" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D164" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D165" t="s">
-        <v>9</v>
-      </c>
-      <c r="E165" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="166" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="167" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="168" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="169" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="170" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C170" t="s">
-        <v>66</v>
+      <c r="D170" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="171" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D172" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D173" t="s">
-        <v>9</v>
-      </c>
-      <c r="E173" t="s">
-        <v>68</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D174" t="s">
-        <v>60</v>
-      </c>
-      <c r="E174" t="s">
-        <v>69</v>
+      <c r="C174" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="175" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="176" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D176" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
     </row>
     <row r="177" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="178" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>9</v>
+      </c>
+      <c r="E177" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="178" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D178" t="s">
+        <v>60</v>
+      </c>
+      <c r="E178" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="179" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D179" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="180" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C180" t="s">
-        <v>128</v>
+      <c r="D180" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="181" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="182" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D182" t="s">
-        <v>129</v>
-      </c>
-      <c r="F182" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="183" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D183" t="s">
-        <v>130</v>
-      </c>
-      <c r="F183" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="184" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D184" t="s">
-        <v>131</v>
-      </c>
-      <c r="F184">
-        <v>0</v>
+      <c r="C184" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="185" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D185" t="s">
-        <v>134</v>
-      </c>
-      <c r="F185" t="b">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="186" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
-        <v>133</v>
-      </c>
-      <c r="F186" t="b">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="F186" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="187" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>135</v>
-      </c>
-      <c r="F187">
-        <v>1</v>
+        <v>130</v>
+      </c>
+      <c r="F187" s="1">
+        <v>0.3</v>
       </c>
     </row>
     <row r="188" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>9</v>
+        <v>134</v>
+      </c>
+      <c r="F189" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
-        <v>13</v>
+        <v>133</v>
+      </c>
+      <c r="F190" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="192" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>135</v>
+      </c>
+      <c r="F191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="194" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C194" t="s">
-        <v>70</v>
+      <c r="D194" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="195" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="196" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D196" t="s">
-        <v>3</v>
-      </c>
-      <c r="E196" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="197" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D197" t="s">
-        <v>72</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="198" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D198" t="s">
-        <v>73</v>
-      </c>
-      <c r="E198" t="s">
-        <v>74</v>
+      <c r="C198" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="199" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>75</v>
-      </c>
-      <c r="E199" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="200" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="E200" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="201" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="202" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D202" t="s">
+        <v>73</v>
+      </c>
+      <c r="E202" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="203" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D203" t="s">
+        <v>75</v>
+      </c>
+      <c r="E203" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="204" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D204" t="s">
+        <v>77</v>
+      </c>
+      <c r="E204" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="205" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D205" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="202" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="206" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add Parking Details Count Entity
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1ACEA3EC-1F6C-4EB2-8EE4-18243703B0BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EF0C4A32-A0E9-4BF2-A27A-BEAB89A05A81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="23610" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="146">
   <si>
     <t>Table Name</t>
   </si>
@@ -433,6 +433,33 @@
   </si>
   <si>
     <t>// Running , Cancel , Parked , Completed</t>
+  </si>
+  <si>
+    <t>parking_details_count</t>
+  </si>
+  <si>
+    <t>park_Loc_id</t>
+  </si>
+  <si>
+    <t>total_count</t>
+  </si>
+  <si>
+    <t>total_occupied</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>booking_cancel_hr</t>
+  </si>
+  <si>
+    <t>advance_booking_hr</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>agent_percentage</t>
   </si>
 </sst>
 </file>
@@ -868,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:I210"/>
+  <dimension ref="C1:I221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,737 +1226,804 @@
     </row>
     <row r="54" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>43</v>
-      </c>
-      <c r="G54" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="62" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>92</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I62" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="63" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>13</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>94</v>
-      </c>
-      <c r="I72" t="s">
-        <v>107</v>
+      <c r="D72" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="74" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>95</v>
-      </c>
-      <c r="F76" t="s">
-        <v>96</v>
+      <c r="C76" t="s">
+        <v>94</v>
+      </c>
+      <c r="I76" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="81" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>108</v>
+      <c r="D81" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>59</v>
-      </c>
-      <c r="I82" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>59</v>
+      </c>
+      <c r="I87" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
+    <row r="89" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>44</v>
-      </c>
-      <c r="I89" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="90" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
-        <v>46</v>
-      </c>
-      <c r="F91" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="92" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>44</v>
+      </c>
+      <c r="I94" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>48</v>
-      </c>
-      <c r="I95" t="s">
-        <v>107</v>
+      <c r="D95" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="F96" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>48</v>
       </c>
-      <c r="E97" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="98" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="99" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="I100" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="101" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>50</v>
-      </c>
-      <c r="E101" t="s">
-        <v>51</v>
+      <c r="D101" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E102" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>53</v>
-      </c>
-      <c r="E104" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="105" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>55</v>
-      </c>
-    </row>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>56</v>
+      <c r="C106" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="107" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="108" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>58</v>
-      </c>
-      <c r="E108" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>15</v>
+        <v>53</v>
+      </c>
+      <c r="E109" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="110" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="113" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>111</v>
+      <c r="D113" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>59</v>
-      </c>
-      <c r="I114" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>24</v>
-      </c>
-    </row>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D118" t="s">
-        <v>3</v>
+      <c r="C118" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>112</v>
-      </c>
-      <c r="F119" t="s">
-        <v>115</v>
+        <v>59</v>
+      </c>
+      <c r="I119" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>120</v>
-      </c>
-      <c r="F121" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="F124" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>15</v>
+        <v>120</v>
+      </c>
+      <c r="F126" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="F129" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
-        <v>126</v>
+      <c r="D130" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>59</v>
-      </c>
-      <c r="I131" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
     </row>
     <row r="132" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>59</v>
+      </c>
+      <c r="I136" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D133" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C137" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="138" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>59</v>
-      </c>
-      <c r="I138" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D140" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
-        <v>120</v>
-      </c>
-      <c r="F141" t="s">
-        <v>125</v>
-      </c>
-    </row>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="140" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D142" t="s">
-        <v>124</v>
+      <c r="C142" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>116</v>
+        <v>59</v>
+      </c>
+      <c r="I143" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
-        <v>9</v>
-      </c>
-      <c r="E144" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
     </row>
     <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>120</v>
+      </c>
+      <c r="F146" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C149" t="s">
-        <v>118</v>
+      <c r="D149" t="s">
+        <v>9</v>
+      </c>
+      <c r="E149" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="150" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>3</v>
-      </c>
-      <c r="I151" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D152" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D153" t="s">
-        <v>120</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="154" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D154" t="s">
-        <v>124</v>
+      <c r="C154" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="155" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
     </row>
     <row r="156" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="I156" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
     </row>
     <row r="158" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="159" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="160" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="162" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="163" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="164" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C165" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D166" t="s">
-        <v>59</v>
+      <c r="C166" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="167" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="H167" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="168" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="169" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>9</v>
-      </c>
-      <c r="E169" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
     </row>
     <row r="170" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="171" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C174" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="175" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D175" t="s">
-        <v>65</v>
-      </c>
-    </row>
+    <row r="174" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D176" t="s">
-        <v>67</v>
+      <c r="C176" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="177" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
-        <v>9</v>
-      </c>
-      <c r="E177" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="178" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>60</v>
-      </c>
-      <c r="E178" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="180" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E180" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="181" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D182" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="183" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C184" t="s">
-        <v>128</v>
-      </c>
-    </row>
+    <row r="184" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="185" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D185" t="s">
-        <v>59</v>
+      <c r="C185" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="186" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
-        <v>129</v>
-      </c>
-      <c r="F186" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>130</v>
-      </c>
-      <c r="F187" s="1">
-        <v>0.3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="188" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>131</v>
-      </c>
-      <c r="F188">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="E188" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="189" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>134</v>
-      </c>
-      <c r="F189" t="b">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="E189" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="190" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
-        <v>133</v>
-      </c>
-      <c r="F190" t="b">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="191" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
-        <v>135</v>
-      </c>
-      <c r="F191">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="192" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D193" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="194" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D194" t="s">
-        <v>13</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="195" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D195" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="196" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="C195" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="196" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="197" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D197" t="s">
+        <v>129</v>
+      </c>
+      <c r="F197" t="s">
+        <v>132</v>
+      </c>
+      <c r="I197" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="198" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C198" t="s">
-        <v>70</v>
+      <c r="D198" t="s">
+        <v>130</v>
+      </c>
+      <c r="F198" s="1">
+        <v>0.3</v>
       </c>
     </row>
     <row r="199" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>59</v>
+        <v>131</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>3</v>
-      </c>
-      <c r="E200" t="s">
-        <v>71</v>
+        <v>134</v>
+      </c>
+      <c r="F200" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>72</v>
+        <v>133</v>
+      </c>
+      <c r="F201" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
-        <v>73</v>
-      </c>
-      <c r="E202" t="s">
-        <v>74</v>
+        <v>135</v>
+      </c>
+      <c r="F202">
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
-        <v>75</v>
-      </c>
-      <c r="E203" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
     </row>
     <row r="204" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
-        <v>77</v>
-      </c>
-      <c r="E204" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="206" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D206" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="207" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="208" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="210" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D210" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="211" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D211" t="s">
+        <v>3</v>
+      </c>
+      <c r="E211" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="212" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D212" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="213" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D213" t="s">
+        <v>73</v>
+      </c>
+      <c r="E213" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="214" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D214" t="s">
+        <v>75</v>
+      </c>
+      <c r="E214" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="215" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D215" t="s">
+        <v>77</v>
+      </c>
+      <c r="E215" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="216" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D216" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="217" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create Entity Referal code and Parking Search location
</commit_message>
<xml_diff>
--- a/docs/parking.xlsx
+++ b/docs/parking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EF0C4A32-A0E9-4BF2-A27A-BEAB89A05A81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D0C6176B-8C8C-406A-8EB4-D439F75978AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="23610" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="23670" windowHeight="16500" activeTab="1" xr2:uid="{2ABAA495-A0BB-4397-9837-811B559CE662}"/>
   </bookViews>
   <sheets>
     <sheet name="Task To do" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="156">
   <si>
     <t>Table Name</t>
   </si>
@@ -234,9 +234,6 @@
     <t>bonus,BB</t>
   </si>
   <si>
-    <t>parking_user_searched_location</t>
-  </si>
-  <si>
     <t>indexed</t>
   </si>
   <si>
@@ -435,9 +432,6 @@
     <t>// Running , Cancel , Parked , Completed</t>
   </si>
   <si>
-    <t>parking_details_count</t>
-  </si>
-  <si>
     <t>park_Loc_id</t>
   </si>
   <si>
@@ -460,6 +454,42 @@
   </si>
   <si>
     <t>agent_percentage</t>
+  </si>
+  <si>
+    <t>parked_vehicle_count</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>referal_code_history</t>
+  </si>
+  <si>
+    <t>referal_userId</t>
+  </si>
+  <si>
+    <t>referee_userId</t>
+  </si>
+  <si>
+    <t>referal_code</t>
+  </si>
+  <si>
+    <t>earn_Money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who is refering </t>
+  </si>
+  <si>
+    <t>referal user</t>
+  </si>
+  <si>
+    <t>parking_searched_location</t>
+  </si>
+  <si>
+    <t>No use</t>
+  </si>
+  <si>
+    <t>This table will save parking search location where our system does not contain any parking location</t>
   </si>
 </sst>
 </file>
@@ -829,7 +859,7 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -837,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -845,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -853,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -861,7 +891,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -869,7 +899,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -877,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -885,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -895,10 +925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80CA144-C390-4A71-ABE0-B5DCEFE76073}">
-  <dimension ref="C1:I221"/>
+  <dimension ref="C1:I227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="G226" sqref="G226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,10 +948,10 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -940,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -1001,7 +1031,7 @@
         <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
@@ -1047,7 +1077,7 @@
         <v>23</v>
       </c>
       <c r="I23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -1078,13 +1108,13 @@
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" t="s">
         <v>88</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>89</v>
-      </c>
-      <c r="G28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
@@ -1099,10 +1129,10 @@
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
@@ -1131,7 +1161,7 @@
         <v>31</v>
       </c>
       <c r="G36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
@@ -1157,7 +1187,7 @@
         <v>34</v>
       </c>
       <c r="I42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
@@ -1200,7 +1230,7 @@
     </row>
     <row r="50" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1213,30 +1243,30 @@
     </row>
     <row r="52" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1244,7 +1274,7 @@
         <v>43</v>
       </c>
       <c r="G57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1259,15 +1289,15 @@
     </row>
     <row r="62" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1277,12 +1307,12 @@
     </row>
     <row r="65" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1292,17 +1322,17 @@
     </row>
     <row r="68" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1322,10 +1352,10 @@
     </row>
     <row r="76" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1335,7 +1365,7 @@
     </row>
     <row r="78" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1345,20 +1375,20 @@
     </row>
     <row r="80" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" t="s">
         <v>95</v>
-      </c>
-      <c r="F80" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="81" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1370,7 +1400,7 @@
     <row r="85" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1378,7 +1408,7 @@
         <v>59</v>
       </c>
       <c r="I87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1423,7 @@
     </row>
     <row r="90" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1408,7 +1438,7 @@
         <v>44</v>
       </c>
       <c r="I94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1436,7 +1466,7 @@
         <v>48</v>
       </c>
       <c r="I100" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1522,7 +1552,7 @@
     <row r="117" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="119" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1530,7 +1560,7 @@
         <v>59</v>
       </c>
       <c r="I119" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1540,7 +1570,7 @@
     </row>
     <row r="121" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="122" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1555,33 +1585,33 @@
     </row>
     <row r="124" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F124" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F126" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="127" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="128" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="129" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1589,12 +1619,12 @@
         <v>9</v>
       </c>
       <c r="F129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1611,7 +1641,7 @@
     <row r="134" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="135" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="136" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1619,7 +1649,7 @@
         <v>59</v>
       </c>
       <c r="I136" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="137" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1629,7 +1659,7 @@
     </row>
     <row r="138" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="139" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1641,7 +1671,7 @@
     <row r="141" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1649,7 +1679,7 @@
         <v>59</v>
       </c>
       <c r="I143" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="144" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1659,25 +1689,25 @@
     </row>
     <row r="145" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F146" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="148" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1702,7 +1732,7 @@
     <row r="153" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="154" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1715,27 +1745,27 @@
         <v>3</v>
       </c>
       <c r="I156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="157" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="160" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1757,176 +1787,173 @@
     <row r="165" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="167" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>138</v>
-      </c>
-      <c r="H167" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="168" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>26</v>
+        <v>136</v>
+      </c>
+      <c r="H168" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="169" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="171" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="172" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="175" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C176" t="s">
+    <row r="176" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="177" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D177" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="178" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="179" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>9</v>
-      </c>
-      <c r="E180" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="181" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>63</v>
+        <v>9</v>
+      </c>
+      <c r="E181" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="182" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="183" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="184" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C185" t="s">
+    <row r="185" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="186" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D186" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="187" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>9</v>
-      </c>
-      <c r="E188" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="189" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E189" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="190" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E190" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="191" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="192" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="194" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C195" t="s">
-        <v>128</v>
-      </c>
-    </row>
+    <row r="195" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="196" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D196" t="s">
-        <v>59</v>
+      <c r="C196" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="197" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
-        <v>129</v>
-      </c>
-      <c r="F197" t="s">
-        <v>132</v>
-      </c>
-      <c r="I197" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
     </row>
     <row r="198" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D198" t="s">
-        <v>130</v>
-      </c>
-      <c r="F198" s="1">
-        <v>0.3</v>
+        <v>128</v>
+      </c>
+      <c r="F198" t="s">
+        <v>131</v>
+      </c>
+      <c r="I198" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="199" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>131</v>
-      </c>
-      <c r="F199">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="F199" s="1">
+        <v>0.3</v>
       </c>
     </row>
     <row r="200" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>134</v>
-      </c>
-      <c r="F200" t="b">
-        <v>1</v>
+        <v>130</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1934,96 +1961,168 @@
         <v>133</v>
       </c>
       <c r="F201" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
-        <v>135</v>
-      </c>
-      <c r="F202">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="F202" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
-        <v>116</v>
+        <v>134</v>
+      </c>
+      <c r="F203">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
     </row>
     <row r="205" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="206" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D207" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="208" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C209" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    <row r="209" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="210" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D210" t="s">
-        <v>59</v>
+      <c r="C210" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="211" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
-        <v>3</v>
-      </c>
-      <c r="E211" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="G211" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="212" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>72</v>
+        <v>3</v>
+      </c>
+      <c r="E212" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="213" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
-        <v>73</v>
-      </c>
-      <c r="E213" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="H213" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="214" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E214" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="G214" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="215" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E215" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="G215" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="216" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D216" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="217" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>76</v>
+      </c>
+      <c r="E216" t="s">
+        <v>77</v>
+      </c>
+      <c r="G216" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="217" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D217" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="218" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D218" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="219" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D219" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="220" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="221" spans="3:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C222" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="223" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D223" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="224" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D224" t="s">
+        <v>147</v>
+      </c>
+      <c r="F224" t="s">
+        <v>151</v>
+      </c>
+      <c r="H224" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="225" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D225" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="226" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
+        <v>150</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="3:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D227" t="s">
+        <v>148</v>
+      </c>
+      <c r="F227" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>